<commit_message>
Fixed modify file uploads and updated test cases
</commit_message>
<xml_diff>
--- a/Deliverables/7. Test Cases/TestCases.xlsx
+++ b/Deliverables/7. Test Cases/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewa_000\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E886E136-9418-4986-8B8D-9B642E370A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAADCD09-7E1F-457D-9FC3-311C71A55047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9FF6808-D506-44CA-A352-BF8FD7553499}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="147">
   <si>
     <t>Test Case</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Logged in as ADMIN</t>
   </si>
   <si>
-    <t>Click on "Modify" in row, complete all form inputs, submit form</t>
-  </si>
-  <si>
     <t>Changes saved, data-table shows updated data</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>ADMIN - Create New Patient Alert</t>
   </si>
   <si>
-    <t>Click on "New" in top right of data-table, complete all form inputs, submit form</t>
-  </si>
-  <si>
     <t>Not logged in</t>
   </si>
   <si>
@@ -472,13 +466,22 @@
   </si>
   <si>
     <t>Appointment is created correctly, but new appointment popup is visually bugged</t>
+  </si>
+  <si>
+    <t>Select entry to modify by pressing "Select" in table</t>
+  </si>
+  <si>
+    <t>Click on "New" in top left of data-table, complete all form inputs, submit form</t>
+  </si>
+  <si>
+    <t>Changed query to update instead of insert in the Modify File Upload section of AdminPanel.java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,8 +519,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +559,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -746,13 +761,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -818,11 +834,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1137,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6347CAB-46C1-4AA1-8DCC-06AF9E9DF055}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,10 +1203,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -1209,38 +1232,38 @@
     </row>
     <row r="4" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="D5" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
@@ -1266,51 +1289,51 @@
     </row>
     <row r="7" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>112</v>
-      </c>
       <c r="D8" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>16</v>
@@ -1323,10 +1346,10 @@
     </row>
     <row r="10" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>17</v>
@@ -1342,114 +1365,114 @@
     </row>
     <row r="11" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="E11" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="E13" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="E14" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="E15" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="E16" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="3"/>
@@ -1462,7 +1485,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>22</v>
@@ -1481,10 +1504,10 @@
         <v>24</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>25</v>
@@ -1532,124 +1555,124 @@
     </row>
     <row r="21" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="D21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>87</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="D23" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="E26" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>33</v>
@@ -1665,38 +1688,38 @@
     </row>
     <row r="28" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1709,23 +1732,23 @@
         <v>36</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>29</v>
@@ -1741,10 +1764,10 @@
     </row>
     <row r="32" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>33</v>
@@ -1758,306 +1781,310 @@
       <c r="F32" s="5"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
     </row>
     <row r="48" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="4"/>

</xml_diff>

<commit_message>
System models and finished test cases
</commit_message>
<xml_diff>
--- a/Deliverables/7. Test Cases/TestCases.xlsx
+++ b/Deliverables/7. Test Cases/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewa_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewa_000\Documents\GitHub\Deliverables\7. Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAADCD09-7E1F-457D-9FC3-311C71A55047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61DFCED-B8A8-466C-900C-416D29EB767F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9FF6808-D506-44CA-A352-BF8FD7553499}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
   <si>
     <t>Test Case</t>
   </si>
@@ -459,9 +459,6 @@
     <t>Shows Old Order popup with diagnostic report</t>
   </si>
   <si>
-    <t>Modality and Estimated Costs do no autofill</t>
-  </si>
-  <si>
     <t>Creates new File Upload rather than modifying the selected upload</t>
   </si>
   <si>
@@ -475,6 +472,15 @@
   </si>
   <si>
     <t>Changed query to update instead of insert in the Modify File Upload section of AdminPanel.java</t>
+  </si>
+  <si>
+    <t>Modified query to return modality and price and populate text fields in AdminPanel.java</t>
+  </si>
+  <si>
+    <t>Entry created, but Modality and Estimated Costs do no autofill</t>
+  </si>
+  <si>
+    <t>Deleted unnecessary fields and rearranged fields in AdminPanel.java to achieve desired appearance</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,6 +844,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1160,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6347CAB-46C1-4AA1-8DCC-06AF9E9DF055}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,7 +1801,7 @@
         <v>38</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>39</v>
@@ -1808,7 +1820,7 @@
         <v>38</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>39</v>
@@ -1827,7 +1839,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>39</v>
@@ -1838,7 +1850,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>43</v>
       </c>
@@ -1846,16 +1858,20 @@
         <v>38</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="3"/>
+        <v>147</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
@@ -1865,16 +1881,16 @@
         <v>38</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G37" s="24" t="s">
         <v>39</v>
@@ -1888,7 +1904,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>39</v>
@@ -1907,7 +1923,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>39</v>
@@ -1926,7 +1942,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>39</v>
@@ -1945,7 +1961,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>39</v>
@@ -1964,7 +1980,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>39</v>
@@ -1975,7 +1991,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>51</v>
       </c>
@@ -1983,16 +1999,20 @@
         <v>38</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
+        <v>142</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
@@ -2002,7 +2022,7 @@
         <v>38</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>39</v>
@@ -2021,7 +2041,7 @@
         <v>38</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>39</v>
@@ -2040,7 +2060,7 @@
         <v>38</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>39</v>
@@ -2059,7 +2079,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>39</v>
@@ -2078,7 +2098,7 @@
         <v>38</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>39</v>

</xml_diff>